<commit_message>
Remove double reading xlsx file in data_only mode for cached formula result
* Cached result and type can be read from cache/cache_type properties of
Cell and ReadOnlyCell
* If cell.is_formula is False, the above properties would both return
None.
</commit_message>
<xml_diff>
--- a/pyxlsx/tests/data/test.xlsx
+++ b/pyxlsx/tests/data/test.xlsx
@@ -8,8 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -365,97 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C1">
-        <f>A1+B1</f>
-        <v/>
-      </c>
-      <c r="D1">
-        <f>vlookup(C1, A1:B4, 2, FALSE)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <f>A2+B2</f>
-        <v/>
-      </c>
-      <c r="D2">
-        <f>vlookup(C2, A1:B4, 2, FALSE)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <f>A3+B3</f>
-        <v/>
-      </c>
-      <c r="D3">
-        <f>vlookup(C3, A1:B4, 2, FALSE)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" t="n">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <f>A4+B4</f>
-        <v/>
-      </c>
-      <c r="D4">
-        <f>vlookup(C4, A1:B4, 2, FALSE)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>demo sample</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,11 +390,6 @@
           <t>int(500)</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>str()</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -513,11 +417,6 @@
           <t>weight</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>origin</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -563,11 +462,6 @@
       </c>
       <c r="E4" t="n">
         <v>1000</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove ReadOnlyCell since it's incompatible with pycel
</commit_message>
<xml_diff>
--- a/pyxlsx/tests/data/test.xlsx
+++ b/pyxlsx/tests/data/test.xlsx
@@ -373,66 +373,44 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr"/>
-      <c r="B1" t="inlineStr"/>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>str('Unknown')</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>float(4.5)</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>int(500)</t>
-        </is>
+      <c r="A1" t="n"/>
+      <c r="B1" t="n"/>
+      <c r="C1" t="n">
+        <v>str('Unknown')</v>
+      </c>
+      <c r="D1" t="n">
+        <v>float(4.5)</v>
+      </c>
+      <c r="E1" t="n">
+        <v>int(500)</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>productName</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>productType</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>weight</t>
-        </is>
+      <c r="A2" t="n">
+        <v>id</v>
+      </c>
+      <c r="B2" t="n">
+        <v>productName</v>
+      </c>
+      <c r="C2" t="n">
+        <v>productType</v>
+      </c>
+      <c r="D2" t="n">
+        <v>price</v>
+      </c>
+      <c r="E2" t="n">
+        <v>weight</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>001</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>pork</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>meat</t>
-        </is>
+      <c r="A3" t="n">
+        <v>001</v>
+      </c>
+      <c r="B3" t="n">
+        <v>pork</v>
+      </c>
+      <c r="C3" t="n">
+        <v>meat</v>
       </c>
       <c r="D3" t="n">
         <v>2.5</v>
@@ -442,20 +420,14 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>002</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>beef</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>meat</t>
-        </is>
+      <c r="A4" t="n">
+        <v>002</v>
+      </c>
+      <c r="B4" t="n">
+        <v>beef</v>
+      </c>
+      <c r="C4" t="n">
+        <v>meat</v>
       </c>
       <c r="D4" t="n">
         <v>4.5</v>

</xml_diff>

<commit_message>
replace original Worksheet with new Worksheet in Workbook' '
</commit_message>
<xml_diff>
--- a/pyxlsx/tests/data/test.xlsx
+++ b/pyxlsx/tests/data/test.xlsx
@@ -373,44 +373,66 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n"/>
-      <c r="B1" t="n"/>
-      <c r="C1" t="n">
-        <v>str('Unknown')</v>
-      </c>
-      <c r="D1" t="n">
-        <v>float(4.5)</v>
-      </c>
-      <c r="E1" t="n">
-        <v>int(500)</v>
+      <c r="A1" t="inlineStr"/>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>str('Unknown')</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>float(4.5)</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>int(500)</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>id</v>
-      </c>
-      <c r="B2" t="n">
-        <v>productName</v>
-      </c>
-      <c r="C2" t="n">
-        <v>productType</v>
-      </c>
-      <c r="D2" t="n">
-        <v>price</v>
-      </c>
-      <c r="E2" t="n">
-        <v>weight</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>productName</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>productType</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>weight</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>001</v>
-      </c>
-      <c r="B3" t="n">
-        <v>pork</v>
-      </c>
-      <c r="C3" t="n">
-        <v>meat</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>001</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>pork</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>meat</t>
+        </is>
       </c>
       <c r="D3" t="n">
         <v>2.5</v>
@@ -420,14 +442,20 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>002</v>
-      </c>
-      <c r="B4" t="n">
-        <v>beef</v>
-      </c>
-      <c r="C4" t="n">
-        <v>meat</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>002</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>beef</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>meat</t>
+        </is>
       </c>
       <c r="D4" t="n">
         <v>4.5</v>

</xml_diff>